<commit_message>
writeToXML.java, now also sets the column size
</commit_message>
<xml_diff>
--- a/graafik.xlsx
+++ b/graafik.xlsx
@@ -35,67 +35,67 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>Daniell/Robert/Madis/Martin/Urmo/Timo/</t>
-  </si>
-  <si>
-    <t>Uku/Madis/Helena/Timo/Helena/Martin/</t>
-  </si>
-  <si>
-    <t>Daniell/Fred/Joel/Kevin/Tanel/Uku/</t>
-  </si>
-  <si>
-    <t>Madis/Fred/Taavi/Robert/Joonas/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Daniell/Buse/Fred/Joonas/Taavi/Helena/</t>
-  </si>
-  <si>
-    <t>Daniell/Siim-Kaarel/Fred/Joel/Helena/Kevin/</t>
-  </si>
-  <si>
-    <t>Joel/Siim-Kaarel/Uku/Daniell/Buse/Kevin/</t>
-  </si>
-  <si>
-    <t>Taavi/Joel/Buse/Fred/Siim/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Rasmus/Deniz/Siim/Buse/Robert/Siim-Kaarel/</t>
-  </si>
-  <si>
-    <t>Rasmus/Siim/Deniz/Siim-Kaarel/Sven-Ervin/Buse/</t>
-  </si>
-  <si>
-    <t>Siim-Kaarel/Timo/Deniz/Martin/Urmo/Siim/</t>
-  </si>
-  <si>
-    <t>Siim/Rasmus/Siim-Sander/Deniz/Anne-Mai/Urmo/</t>
-  </si>
-  <si>
-    <t>Tanel/Anne-Mai/Madis/Rasmus/Triinu/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Madis/Helena/Tanel/Joonas/Rasmus/Urmo/</t>
-  </si>
-  <si>
-    <t>Anne-Mai/Triinu/Sven-Ervin/</t>
-  </si>
-  <si>
-    <t>Urmo/Joonas/Taavi/</t>
-  </si>
-  <si>
-    <t>Anne-Mai/Helena/Helena/</t>
-  </si>
-  <si>
-    <t>Joel/Triinu/Kevin/</t>
-  </si>
-  <si>
-    <t>Robert/Uku/Helena/</t>
-  </si>
-  <si>
-    <t>Taavi/Sven-Ervin/Martin/</t>
-  </si>
-  <si>
-    <t>Robert/Anne-Mai/Siim-Sander/</t>
+    <t>Siim/Joel/Helena/Taavi/Siim/Robert/</t>
+  </si>
+  <si>
+    <t>Rasmus/Siim/Joel/Siim/Anne-Mai/Deniz/</t>
+  </si>
+  <si>
+    <t>Siim/Fred/Taavi/Anne-Mai/Siim/Kevin/</t>
+  </si>
+  <si>
+    <t>Timo/Uku/Deniz/Siim/Siim-Sander/Tanel/</t>
+  </si>
+  <si>
+    <t>Marko/Deniz/Siim-Kaarel/Kevin/Siim-Sander/Siim/</t>
+  </si>
+  <si>
+    <t>Fred/Siim-Sander/Siim-Kaarel/Robert/Siim/Helena/</t>
+  </si>
+  <si>
+    <t>Helena/Sven-Ervin/Robert/Joonas/Kevin/Fred/</t>
+  </si>
+  <si>
+    <t>Madis/Joonas/Fred/Urmo/Helena/Kevin/</t>
+  </si>
+  <si>
+    <t>Joonas/Siim-Kaarel/Uku/Helena/Robert/Madis/</t>
+  </si>
+  <si>
+    <t>Helena/Siim-Kaarel/Joonas/Martin/Joel/Helena/</t>
+  </si>
+  <si>
+    <t>Martin/Robert/Taavi/Daniell/Urmo/Joel/</t>
+  </si>
+  <si>
+    <t>Martin/Taavi/Joel/Urmo/Helena/Tanel/</t>
+  </si>
+  <si>
+    <t>Timo/Helena/Marko/Taavi/Madis/Urmo/</t>
+  </si>
+  <si>
+    <t>Deniz/Urmo/Siim-Kaarel/Marko/Anne-Mai/Timo/</t>
+  </si>
+  <si>
+    <t>Marko/Martin/Sven-Ervin/</t>
+  </si>
+  <si>
+    <t>Tanel/Daniell/Siim-Sander/</t>
+  </si>
+  <si>
+    <t>Madis/Sven-Ervin/Triinu/</t>
+  </si>
+  <si>
+    <t>Helena/Rasmus/Siim/</t>
+  </si>
+  <si>
+    <t>Anne-Mai/Sven-Ervin/Joonas/</t>
+  </si>
+  <si>
+    <t>Rasmus/Martin/Tanel/</t>
+  </si>
+  <si>
+    <t>Siim-Sander/Daniell/Madis/</t>
   </si>
 </sst>
 </file>
@@ -145,6 +145,15 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="37.9375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="43.66796875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="44.37109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="38.48828125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="46.3671875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="47.046875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="45.390625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="2">
       <c r="B2" t="s">

</xml_diff>

<commit_message>
readFromXML.java the file name can now be set
</commit_message>
<xml_diff>
--- a/graafik.xlsx
+++ b/graafik.xlsx
@@ -35,67 +35,67 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>Siim/Joel/Helena/Taavi/Siim/Robert/</t>
-  </si>
-  <si>
-    <t>Rasmus/Siim/Joel/Siim/Anne-Mai/Deniz/</t>
-  </si>
-  <si>
-    <t>Siim/Fred/Taavi/Anne-Mai/Siim/Kevin/</t>
-  </si>
-  <si>
-    <t>Timo/Uku/Deniz/Siim/Siim-Sander/Tanel/</t>
-  </si>
-  <si>
-    <t>Marko/Deniz/Siim-Kaarel/Kevin/Siim-Sander/Siim/</t>
-  </si>
-  <si>
-    <t>Fred/Siim-Sander/Siim-Kaarel/Robert/Siim/Helena/</t>
-  </si>
-  <si>
-    <t>Helena/Sven-Ervin/Robert/Joonas/Kevin/Fred/</t>
-  </si>
-  <si>
-    <t>Madis/Joonas/Fred/Urmo/Helena/Kevin/</t>
-  </si>
-  <si>
-    <t>Joonas/Siim-Kaarel/Uku/Helena/Robert/Madis/</t>
-  </si>
-  <si>
-    <t>Helena/Siim-Kaarel/Joonas/Martin/Joel/Helena/</t>
-  </si>
-  <si>
-    <t>Martin/Robert/Taavi/Daniell/Urmo/Joel/</t>
-  </si>
-  <si>
-    <t>Martin/Taavi/Joel/Urmo/Helena/Tanel/</t>
-  </si>
-  <si>
-    <t>Timo/Helena/Marko/Taavi/Madis/Urmo/</t>
-  </si>
-  <si>
-    <t>Deniz/Urmo/Siim-Kaarel/Marko/Anne-Mai/Timo/</t>
-  </si>
-  <si>
-    <t>Marko/Martin/Sven-Ervin/</t>
-  </si>
-  <si>
-    <t>Tanel/Daniell/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Madis/Sven-Ervin/Triinu/</t>
-  </si>
-  <si>
-    <t>Helena/Rasmus/Siim/</t>
-  </si>
-  <si>
-    <t>Anne-Mai/Sven-Ervin/Joonas/</t>
-  </si>
-  <si>
-    <t>Rasmus/Martin/Tanel/</t>
-  </si>
-  <si>
-    <t>Siim-Sander/Daniell/Madis/</t>
+    <t>Triinu/Joel/Uku/Siim/Rasmus/Fred/</t>
+  </si>
+  <si>
+    <t>Rasmus/Tanel/Martin/Robert/Siim/Helena/</t>
+  </si>
+  <si>
+    <t>Siim-Sander/Taavi/Fred/Timo/Kevin/Deniz/</t>
+  </si>
+  <si>
+    <t>Fred/Robert/Sven-Ervin/Timo/Rasmus/Siim-Kaarel/</t>
+  </si>
+  <si>
+    <t>Daniell/Helena/Siim-Sander/Marko/Sven-Ervin/Kevin/</t>
+  </si>
+  <si>
+    <t>Daniell/Madis/Uku/Siim/Triinu/Sven-Ervin/</t>
+  </si>
+  <si>
+    <t>Martin/Siim/Taavi/Anne-Mai/Madis/Robert/</t>
+  </si>
+  <si>
+    <t>Marko/Sven-Ervin/Taavi/Timo/Siim-Kaarel/Deniz/</t>
+  </si>
+  <si>
+    <t>Marko/Helena/Siim-Kaarel/Joel/Uku/Triinu/</t>
+  </si>
+  <si>
+    <t>Martin/Helena/Madis/Uku/Siim/Helena/</t>
+  </si>
+  <si>
+    <t>Anne-Mai/Urmo/Siim/Joonas/Joel/Taavi/</t>
+  </si>
+  <si>
+    <t>Urmo/Joel/Rasmus/Taavi/Siim/Tanel/</t>
+  </si>
+  <si>
+    <t>Urmo/Siim/Fred/Helena/Kevin/Helena/</t>
+  </si>
+  <si>
+    <t>Marko/Timo/Urmo/Daniell/Helena/Siim-Kaarel/</t>
+  </si>
+  <si>
+    <t>Siim-Sander/Madis/Daniell/</t>
+  </si>
+  <si>
+    <t>Joonas/Sven-Ervin/Siim/</t>
+  </si>
+  <si>
+    <t>Tanel/Marko/Triinu/</t>
+  </si>
+  <si>
+    <t>Siim/Helena/Uku/</t>
+  </si>
+  <si>
+    <t>Robert/Martin/Timo/</t>
+  </si>
+  <si>
+    <t>Siim-Sander/Rasmus/Tanel/</t>
+  </si>
+  <si>
+    <t>Triinu/Deniz/Fred/</t>
   </si>
 </sst>
 </file>
@@ -146,13 +146,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="37.9375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="43.66796875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="44.37109375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="38.48828125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="46.3671875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="47.046875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="45.390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="45.60546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="40.4921875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="39.859375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="47.10546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="49.4140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="39.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="44.06640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">

</xml_diff>

<commit_message>
Parser.parse, removed infinite loop situations, will give half-baked shifthseet if neccessary writeToXML.writeInput now also inputs info about people who didn't get 40 hours, and file location can be changed from the test file
</commit_message>
<xml_diff>
--- a/graafik.xlsx
+++ b/graafik.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Graafik" r:id="rId3" sheetId="1"/>
+    <sheet name="Shift" r:id="rId3" sheetId="1"/>
+    <sheet name="People with under 40 hours" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Monday</t>
   </si>
@@ -35,67 +36,97 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>Timo/Madis/Tanel/Urmo/Helena/Triinu/</t>
-  </si>
-  <si>
-    <t>Helena/Joel/Uku/Marko/Siim/Urmo/</t>
-  </si>
-  <si>
-    <t>Joel/Helena/Siim/Marko/Kevin/Deniz/</t>
-  </si>
-  <si>
-    <t>Timo/Urmo/Sven-Ervin/Tanel/Rasmus/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Fred/Rasmus/Triinu/Sven-Ervin/Marko/Taavi/</t>
-  </si>
-  <si>
-    <t>Siim/Taavi/Daniell/Madis/Martin/Anne-Mai/</t>
-  </si>
-  <si>
-    <t>Robert/Rasmus/Deniz/Taavi/Anne-Mai/Siim/</t>
-  </si>
-  <si>
-    <t>Siim-Kaarel/Taavi/Helena/Sven-Ervin/Fred/Deniz/</t>
-  </si>
-  <si>
-    <t>Madis/Joonas/Triinu/Rasmus/Martin/Helena/</t>
-  </si>
-  <si>
-    <t>Madis/Fred/Joonas/Anne-Mai/Martin/Helena/</t>
-  </si>
-  <si>
-    <t>Madis/Joel/Helena/Helena/Uku/Daniell/</t>
-  </si>
-  <si>
-    <t>Joel/Urmo/Siim/Siim-Kaarel/Helena/Siim-Sander/</t>
-  </si>
-  <si>
-    <t>Marko/Kevin/Fred/Urmo/Siim/Sven-Ervin/</t>
-  </si>
-  <si>
-    <t>Timo/Daniell/Fred/Siim/Martin/Marko/</t>
-  </si>
-  <si>
-    <t>Siim/Kevin/Anne-Mai/</t>
-  </si>
-  <si>
-    <t>Tanel/Sven-Ervin/Timo/</t>
-  </si>
-  <si>
-    <t>Siim/Taavi/Robert/</t>
-  </si>
-  <si>
-    <t>Kevin/Joonas/Martin/</t>
-  </si>
-  <si>
-    <t>Helena/Timo/Uku/</t>
-  </si>
-  <si>
-    <t>Joel/Siim-Sander/Siim-Kaarel/</t>
-  </si>
-  <si>
-    <t>Uku/Kevin/Triinu/</t>
+    <t>Buse/Martin/Anne-Mai/Daniell/Rasmus/Deniz/</t>
+  </si>
+  <si>
+    <t>Martin/Uku/Timo/Siim-Kaarel/Anne-Mai/Deniz/</t>
+  </si>
+  <si>
+    <t>Urmo/Uku/Kevin/Helena/Anne-Mai/Daniell/</t>
+  </si>
+  <si>
+    <t>Robert/Taavi/Fred/Madis/Daniell/Kevin/</t>
+  </si>
+  <si>
+    <t>Robert/Urmo/Deniz/Joel/Rasmus/Uku/</t>
+  </si>
+  <si>
+    <t>Joel/Siim-Sander/Tanel/Siim/Triinu/Rasmus/</t>
+  </si>
+  <si>
+    <t>Helena/Uku/Triinu/Siim/Joonas/Joel/</t>
+  </si>
+  <si>
+    <t>Fred/Madis/Sven-Ervin/Tanel/Robert/Joel/</t>
+  </si>
+  <si>
+    <t>Madis/Buse/Robert/Rasmus/Sven-Ervin/Siim/</t>
+  </si>
+  <si>
+    <t>Sven-Ervin/Siim-Kaarel/Tanel/Rasmus/Siim/Triinu/</t>
+  </si>
+  <si>
+    <t>Siim/Sven-Ervin/Tanel/Timo/Triinu/Siim-Kaarel/</t>
+  </si>
+  <si>
+    <t>Daniell/Madis/Taavi/Siim-Kaarel/Anne-Mai/Sven-Ervin/</t>
+  </si>
+  <si>
+    <t>Kevin/Madis/Fred/Robert/Anne-Mai/Taavi/</t>
+  </si>
+  <si>
+    <t>Buse/Siim-Kaarel/Kevin/Taavi/Siim-Sander/Tanel/</t>
+  </si>
+  <si>
+    <t>Helena/Siim-Sander/Triinu/</t>
+  </si>
+  <si>
+    <t>Joel/Fred/Taavi/</t>
+  </si>
+  <si>
+    <t>Deniz/Joonas/Helena/</t>
+  </si>
+  <si>
+    <t>Siim-Sander/Buse/Martin/</t>
+  </si>
+  <si>
+    <t>Helena/Joonas/Helena/</t>
+  </si>
+  <si>
+    <t>Martin/Daniell/Urmo/</t>
+  </si>
+  <si>
+    <t>FredK/</t>
+  </si>
+  <si>
+    <t>Joonas</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>Deniz</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Siim-Sander</t>
+  </si>
+  <si>
+    <t>Uku</t>
+  </si>
+  <si>
+    <t>Buse</t>
+  </si>
+  <si>
+    <t>Urmo</t>
+  </si>
+  <si>
+    <t>Kevin</t>
   </si>
 </sst>
 </file>
@@ -146,13 +177,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="45.55078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="42.0625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="42.84375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="47.56640625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="45.46875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="41.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="41.31640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="43.33203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="44.1015625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="46.29296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="43.90625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="50.69140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="40.953125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="45.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -247,7 +278,163 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19">
+      <c r="B19"/>
+      <c r="C19"/>
+    </row>
+    <row r="20">
+      <c r="B20"/>
+      <c r="C20"/>
+    </row>
+    <row r="21">
+      <c r="B21"/>
+      <c r="C21"/>
+    </row>
+    <row r="22">
+      <c r="B22"/>
+      <c r="C22"/>
+    </row>
+    <row r="23">
+      <c r="B23"/>
+      <c r="C23"/>
+    </row>
+    <row r="24">
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25">
+      <c r="B25"/>
+      <c r="C25"/>
+    </row>
+    <row r="26">
+      <c r="B26"/>
+      <c r="C26"/>
+    </row>
+    <row r="27">
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28">
+      <c r="B28"/>
+      <c r="C28"/>
+    </row>
+    <row r="29">
+      <c r="B29"/>
+      <c r="C29"/>
+    </row>
+    <row r="30">
+      <c r="B30"/>
+      <c r="C30"/>
+    </row>
+    <row r="31">
+      <c r="B31"/>
+      <c r="C31"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All names now have the first letter of their last name added.
</commit_message>
<xml_diff>
--- a/graafik.xlsx
+++ b/graafik.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Monday</t>
   </si>
@@ -36,97 +36,100 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>Buse/Martin/Anne-Mai/Daniell/Rasmus/Deniz/</t>
-  </si>
-  <si>
-    <t>Martin/Uku/Timo/Siim-Kaarel/Anne-Mai/Deniz/</t>
-  </si>
-  <si>
-    <t>Urmo/Uku/Kevin/Helena/Anne-Mai/Daniell/</t>
-  </si>
-  <si>
-    <t>Robert/Taavi/Fred/Madis/Daniell/Kevin/</t>
-  </si>
-  <si>
-    <t>Robert/Urmo/Deniz/Joel/Rasmus/Uku/</t>
-  </si>
-  <si>
-    <t>Joel/Siim-Sander/Tanel/Siim/Triinu/Rasmus/</t>
-  </si>
-  <si>
-    <t>Helena/Uku/Triinu/Siim/Joonas/Joel/</t>
-  </si>
-  <si>
-    <t>Fred/Madis/Sven-Ervin/Tanel/Robert/Joel/</t>
-  </si>
-  <si>
-    <t>Madis/Buse/Robert/Rasmus/Sven-Ervin/Siim/</t>
-  </si>
-  <si>
-    <t>Sven-Ervin/Siim-Kaarel/Tanel/Rasmus/Siim/Triinu/</t>
-  </si>
-  <si>
-    <t>Siim/Sven-Ervin/Tanel/Timo/Triinu/Siim-Kaarel/</t>
-  </si>
-  <si>
-    <t>Daniell/Madis/Taavi/Siim-Kaarel/Anne-Mai/Sven-Ervin/</t>
-  </si>
-  <si>
-    <t>Kevin/Madis/Fred/Robert/Anne-Mai/Taavi/</t>
-  </si>
-  <si>
-    <t>Buse/Siim-Kaarel/Kevin/Taavi/Siim-Sander/Tanel/</t>
-  </si>
-  <si>
-    <t>Helena/Siim-Sander/Triinu/</t>
-  </si>
-  <si>
-    <t>Joel/Fred/Taavi/</t>
-  </si>
-  <si>
-    <t>Deniz/Joonas/Helena/</t>
-  </si>
-  <si>
-    <t>Siim-Sander/Buse/Martin/</t>
-  </si>
-  <si>
-    <t>Helena/Joonas/Helena/</t>
-  </si>
-  <si>
-    <t>Martin/Daniell/Urmo/</t>
-  </si>
-  <si>
-    <t>FredK/</t>
-  </si>
-  <si>
-    <t>Joonas</t>
-  </si>
-  <si>
-    <t>Helena</t>
-  </si>
-  <si>
-    <t>Timo</t>
-  </si>
-  <si>
-    <t>Deniz</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Siim-Sander</t>
-  </si>
-  <si>
-    <t>Uku</t>
-  </si>
-  <si>
-    <t>Buse</t>
-  </si>
-  <si>
-    <t>Urmo</t>
-  </si>
-  <si>
-    <t>Kevin</t>
+    <t>BuseE/MartinM/UrmoO/RobertM/MadisK/HelenaM/</t>
+  </si>
+  <si>
+    <t>DaniellS/UkuJ/UrmoO/MartinM/BuseE/Anne-MaiP/</t>
+  </si>
+  <si>
+    <t>Anne-MaiP/TanelM/TaaviP/Sven-ErvinP/TriinuS/DaniellS/</t>
+  </si>
+  <si>
+    <t>TanelM/KevinV/Anne-MaiP/DaniellS/JoelK/JoonasK/</t>
+  </si>
+  <si>
+    <t>HelenaJ/HelenaM/UkuJ/JoelK/UrmoO/RasmusR/</t>
+  </si>
+  <si>
+    <t>JoonasK/JoelK/FredK/Sven-ErvinP/RasmusR/HelenaM/</t>
+  </si>
+  <si>
+    <t>RasmusR/TriinuS/Siim-KaarelK/Anne-MaiP/KevinV/JoonasK/</t>
+  </si>
+  <si>
+    <t>FredK/Sven-ErvinP/TanelM/SiimL/JoelK/DenizG/</t>
+  </si>
+  <si>
+    <t>RobertM/MadisK/DenizG/SiimL/RasmusR/TimoK/</t>
+  </si>
+  <si>
+    <t>UkuJ/MadisK/UrmoO/FredK/SiimL/RasmusR/</t>
+  </si>
+  <si>
+    <t>MadisK/TriinuS/SiimL/Siim-KaarelK/TaaviP/TimoK/</t>
+  </si>
+  <si>
+    <t>DaniellS/Anne-MaiP/TaaviP/DenizG/BuseE/Siim-SanderS/</t>
+  </si>
+  <si>
+    <t>Siim-SanderS/TanelM/DaniellS/RobertM/MadisK/UrmoO/</t>
+  </si>
+  <si>
+    <t>Siim-SanderS/Sven-ErvinP/UkuJ/TanelM/FredK/RobertM/</t>
+  </si>
+  <si>
+    <t>Siim-SanderS/TaaviP/Siim-KaarelK/</t>
+  </si>
+  <si>
+    <t>JoonasK/HelenaM/KevinV/</t>
+  </si>
+  <si>
+    <t>DenizG/Siim-SanderS/BuseE/</t>
+  </si>
+  <si>
+    <t>RobertM/MartinM/FredK/</t>
+  </si>
+  <si>
+    <t>KevinV/SiimL/TriinuS/</t>
+  </si>
+  <si>
+    <t>MartinM/HelenaJ/TaaviP/</t>
+  </si>
+  <si>
+    <t>BuseE/JoelK/</t>
+  </si>
+  <si>
+    <t>Sven-ErvinP</t>
+  </si>
+  <si>
+    <t>JoonasK</t>
+  </si>
+  <si>
+    <t>HelenaM</t>
+  </si>
+  <si>
+    <t>TimoK</t>
+  </si>
+  <si>
+    <t>DenizG</t>
+  </si>
+  <si>
+    <t>MartinM</t>
+  </si>
+  <si>
+    <t>TriinuS</t>
+  </si>
+  <si>
+    <t>Siim-KaarelK</t>
+  </si>
+  <si>
+    <t>UkuJ</t>
+  </si>
+  <si>
+    <t>KevinV</t>
+  </si>
+  <si>
+    <t>HelenaJ</t>
   </si>
 </sst>
 </file>
@@ -177,13 +180,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="43.33203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="44.1015625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="46.29296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="43.90625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="50.69140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="40.953125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="45.6171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="48.7578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="47.39453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="52.51953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="47.953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="52.47265625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="52.88671875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="54.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -283,7 +286,7 @@
         <v>28</v>
       </c>
       <c r="C7" t="n">
-        <v>24.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="8">
@@ -291,7 +294,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="n">
-        <v>16.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="9">
@@ -299,7 +302,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>16.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="10">
@@ -307,7 +310,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="n">
-        <v>32.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="11">
@@ -339,7 +342,7 @@
         <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>32.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="15">
@@ -347,7 +350,7 @@
         <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>24.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="16">
@@ -360,10 +363,10 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C17" t="n">
-        <v>32.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="18">

</xml_diff>